<commit_message>
Update Review Comments Documents.xlsx
</commit_message>
<xml_diff>
--- a/PM/PMP/Review Comments Documents.xlsx
+++ b/PM/PMP/Review Comments Documents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1-ITI\15- Quality Assurance\1- Workshop\1- GIT\GitHub\learning-hub\PM\PMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2F0661-4513-441F-A624-5066E6DBBECA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F6F46A-0C02-4CB0-9358-FDE4A177E24A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{517ADA08-9008-4EF8-8B33-926C871191B2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t xml:space="preserve">PMP - Review Comments </t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t xml:space="preserve">Baseline Strategy </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -166,20 +172,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="6" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -246,7 +244,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -269,6 +267,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -278,37 +296,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165473DF-4415-4360-A898-B8D88BBC8B39}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,21 +658,23 @@
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -676,364 +696,413 @@
       <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="H2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="G4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="G7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="G8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="G10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="6">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="G11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="G12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
-        <v>11</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="7">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>45202</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="G14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>12</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>45202</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="G15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>13</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>45202</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="G16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>14</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>45202</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="E17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>15</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>45202</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>11</v>
+      <c r="G18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>